<commit_message>
new serial port and new protocol added to code
</commit_message>
<xml_diff>
--- a/Documentation/Panel KeyBoard Layout.xlsx
+++ b/Documentation/Panel KeyBoard Layout.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ambition\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Mobin3\Mobin3_src\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="0" windowWidth="27180" windowHeight="14715"/>
+    <workbookView xWindow="4410" yWindow="0" windowWidth="27180" windowHeight="14715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Keys" sheetId="1" r:id="rId1"/>
@@ -385,12 +385,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -402,25 +420,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,7 +705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -935,10 +936,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,228 +950,223 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>30</v>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B8" s="6" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>39</v>
+      <c r="A11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>40</v>
+      <c r="A12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>41</v>
+      <c r="A13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>42</v>
+      <c r="A14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>43</v>
+      <c r="A15" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>44</v>
+      <c r="A16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>45</v>
+      <c r="A17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>46</v>
+      <c r="A18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>47</v>
+      <c r="A19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>49</v>
+      <c r="A20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>50</v>
+      <c r="A21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>51</v>
+      <c r="A22" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>52</v>
+      <c r="A23" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>53</v>
+      <c r="A24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>54</v>
+      <c r="A25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>48</v>
+      <c r="A26" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>55</v>
+      <c r="A27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>56</v>
+      <c r="A28" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A29" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B29" s="8" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1202,87 +1198,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
keyboard feedback protocol added to user interface
</commit_message>
<xml_diff>
--- a/Documentation/Panel KeyBoard Layout.xlsx
+++ b/Documentation/Panel KeyBoard Layout.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
   <si>
     <t>#</t>
   </si>
@@ -233,6 +233,15 @@
   <si>
     <t>0x00: OFF 
 0x01: ON</t>
+  </si>
+  <si>
+    <t>Byte 6</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>0x00</t>
   </si>
 </sst>
 </file>
@@ -411,6 +420,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -419,9 +431,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -936,10 +945,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,11 +959,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -964,7 +973,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="81" customHeight="1" x14ac:dyDescent="0.25">
@@ -990,7 +999,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1004,169 +1013,177 @@
     </row>
     <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B30" s="8" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1184,7 +1201,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1198,15 +1215,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1228,7 +1245,7 @@
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">

</xml_diff>